<commit_message>
Mod bumps for RO v6 a6
Mod bumps, plus four new mods
</commit_message>
<xml_diff>
--- a/Mods (26:7:14 0600).xlsx
+++ b/Mods (26:7:14 0600).xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="44600" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28800" windowHeight="12380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="109">
   <si>
     <t>home</t>
   </si>
@@ -75,9 +75,6 @@
     <t>http://forum.kerbalspaceprogram.com/threads/84689</t>
   </si>
   <si>
-    <t>https://github.com/NathanKell/RealismOverhaul/releases/download/v6.0a5/RealismOverhaul-6.0a5.zip</t>
-  </si>
-  <si>
     <t>A set of patches that resizes and reconfigures parts to resemble realistic technology</t>
   </si>
   <si>
@@ -283,6 +280,72 @@
   </si>
   <si>
     <t>https://www.dropbox.com/s/yousr4nxflld9ra/EngineIgnitor%20V3.2.zip?dl=1</t>
+  </si>
+  <si>
+    <t>Crossfeed Enabler</t>
+  </si>
+  <si>
+    <t>Kerbal Joint Reinforcement</t>
+  </si>
+  <si>
+    <t>Mechjeb</t>
+  </si>
+  <si>
+    <t>PartCatalog</t>
+  </si>
+  <si>
+    <t>Automatically enables crossfeed on radial tanks</t>
+  </si>
+  <si>
+    <t>Makes joint connections more realistic, as well as preventing physics jumps</t>
+  </si>
+  <si>
+    <t>An all in one autopilot and information mod.</t>
+  </si>
+  <si>
+    <t>Tired of scrolling through page after page of parts? PartCatalog is the answer.</t>
+  </si>
+  <si>
+    <t>2.1.7</t>
+  </si>
+  <si>
+    <t>http://forum.kerbalspaceprogram.com/threads/76499</t>
+  </si>
+  <si>
+    <t>https://github.com/NathanKell/CrossFeedEnabler/releases/download/v2.2/CrossFeedEnabler_v2.2.zip</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/11467249/PartCatalog/PartCatalog3.0_RC5.zip</t>
+  </si>
+  <si>
+    <t>http://forum.kerbalspaceprogram.com/threads/35018</t>
+  </si>
+  <si>
+    <t>3.0.5</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t>http://forum.kerbalspaceprogram.com/threads/12384</t>
+  </si>
+  <si>
+    <t>http://www.curse.com/ksp-mods/kerbal/220221-mechjeb/2209611#</t>
+  </si>
+  <si>
+    <t>http://forum.kerbalspaceprogram.com/threads/55657</t>
+  </si>
+  <si>
+    <t>2.4.3</t>
+  </si>
+  <si>
+    <t>https://github.com/ferram4/Kerbal-Joint-Reinforcement/releases/download/v2.4.3/KerbalJointReinforcement_v2.4.3.zip</t>
+  </si>
+  <si>
+    <t>https://github.com/NathanKell/RealismOverhaul/releases/download/v6.0a6.2/RealismOverhaulv6.0a6.2.zip</t>
+  </si>
+  <si>
+    <t>6.0.61</t>
   </si>
 </sst>
 </file>
@@ -350,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -422,8 +485,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -639,8 +737,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -674,8 +776,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="219">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -783,6 +888,8 @@
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -890,6 +997,8 @@
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1219,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="102" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1279,7 +1388,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="5"/>
@@ -1374,10 +1483,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5">
-        <v>6.05</v>
+        <v>107</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="F4" s="12" t="b">
         <v>1</v>
@@ -1386,7 +1495,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="13"/>
       <c r="M4" s="14" t="b">
@@ -1407,7 +1516,7 @@
     </row>
     <row r="5" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
@@ -1416,7 +1525,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -1428,10 +1537,10 @@
         <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" s="15"/>
       <c r="M5" s="16" t="b">
@@ -1452,7 +1561,7 @@
     </row>
     <row r="6" spans="1:25" s="19" customFormat="1" ht="15" thickBot="1">
       <c r="A6" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>14</v>
@@ -1461,7 +1570,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="19">
         <v>1</v>
@@ -1473,10 +1582,10 @@
         <v>13</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="21" t="b">
@@ -1497,7 +1606,7 @@
     </row>
     <row r="7" spans="1:25" s="19" customFormat="1" ht="15" thickBot="1">
       <c r="A7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>14</v>
@@ -1506,7 +1615,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="19">
         <v>1</v>
@@ -1518,10 +1627,10 @@
         <v>13</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7" s="20"/>
       <c r="M7" s="21" t="b">
@@ -1569,16 +1678,16 @@
     </row>
     <row r="9" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="2">
         <v>7.1</v>
@@ -1587,10 +1696,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="24" t="b">
@@ -1611,16 +1720,16 @@
     </row>
     <row r="10" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2">
         <v>5.2</v>
@@ -1629,10 +1738,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="23"/>
       <c r="M10" s="24" t="b">
@@ -1653,16 +1762,16 @@
     </row>
     <row r="11" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="2">
         <v>14.11</v>
@@ -1671,10 +1780,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L11" s="23"/>
       <c r="M11" s="24" t="b">
@@ -1695,16 +1804,16 @@
     </row>
     <row r="12" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2">
         <v>1.22</v>
@@ -1713,10 +1822,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L12" s="23"/>
       <c r="M12" s="16" t="b">
@@ -1737,16 +1846,16 @@
     </row>
     <row r="13" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="2">
         <v>3.21</v>
@@ -1755,10 +1864,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="16" t="b">
@@ -1779,16 +1888,16 @@
     </row>
     <row r="14" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2">
         <v>0.3</v>
@@ -1797,10 +1906,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="16" t="b">
@@ -1821,16 +1930,16 @@
     </row>
     <row r="15" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" s="2">
         <v>1.4</v>
@@ -1839,10 +1948,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="24" t="b">
@@ -1863,16 +1972,16 @@
     </row>
     <row r="16" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -1881,13 +1990,13 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="L16" s="17"/>
       <c r="M16" s="16" t="b">
@@ -1935,16 +2044,16 @@
     </row>
     <row r="18" spans="1:25" s="5" customFormat="1" ht="15" thickBot="1">
       <c r="A18" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" s="26">
         <v>1.32</v>
@@ -1953,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="26" t="s">
         <v>69</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>70</v>
       </c>
       <c r="L18" s="13"/>
       <c r="M18" s="14" t="b">
@@ -1977,16 +2086,16 @@
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" ht="15" thickBot="1">
       <c r="A19" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" s="26">
         <v>0.91500000000000004</v>
@@ -1995,10 +2104,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="14" t="b">
@@ -2019,16 +2128,16 @@
     </row>
     <row r="20" spans="1:25" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A20" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20" s="28">
         <v>1.4</v>
@@ -2037,10 +2146,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L20" s="17"/>
       <c r="M20" s="24" t="b">
@@ -2061,16 +2170,16 @@
     </row>
     <row r="21" spans="1:25" s="19" customFormat="1" ht="15" thickBot="1">
       <c r="A21" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>79</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>80</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" s="30">
         <v>3.08</v>
@@ -2079,10 +2188,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L21" s="22"/>
       <c r="M21" s="21" t="b">
@@ -2103,16 +2212,16 @@
     </row>
     <row r="22" spans="1:25" s="19" customFormat="1" ht="15" thickBot="1">
       <c r="A22" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E22" s="30">
         <v>0.93</v>
@@ -2121,10 +2230,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L22" s="22"/>
       <c r="M22" s="21" t="b">
@@ -2143,33 +2252,160 @@
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
     </row>
-    <row r="23" spans="1:25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="6"/>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="H24" s="31"/>
-    </row>
-    <row r="25" spans="1:25">
-      <c r="A25" s="10" t="e">
-        <f>- name: Real Solar System</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H25" s="10" t="s">
+    <row r="23" spans="1:25" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A23" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="33" t="b">
         <v>0</v>
       </c>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:25" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A24" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="1:25" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A25" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" s="8"/>
+    </row>
+    <row r="26" spans="1:25" s="9" customFormat="1" ht="15" thickBot="1">
+      <c r="A26" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="H28" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>